<commit_message>
add new products and ideas
</commit_message>
<xml_diff>
--- a/data/s.xlsx
+++ b/data/s.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylezhang/Documents/Agora.io/Code/Idea-Box/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylezhang/Library/Containers/com.tencent.WeWorkMac/Data/Documents/Profiles/D1CB5E35BC754BAAFAA950D940E522EC/Caches/Files/2022-09/d8ed1ee94000db0fedb4201f756ded1d/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AEB102-9501-074F-8703-B4842AFCF602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5956B1CA-6914-DC40-8CD3-55E724A72EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="760" windowWidth="29340" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15540" yWindow="760" windowWidth="14680" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="305">
   <si>
     <t>1v1 教学</t>
   </si>
@@ -702,9 +702,6 @@
     <t>声网视频通话 API｜https://www.agora.io/cn/videocall</t>
   </si>
   <si>
-    <t>微光｜http://www.vlightv.com/</t>
-  </si>
-  <si>
     <t>窝窝｜https://www.wewave.com.cn/</t>
   </si>
   <si>
@@ -744,9 +741,6 @@
     <t>开源项目 Obs Studio｜https://github.com/obsproject/obs-studio</t>
   </si>
   <si>
-    <t>Cmeeting｜https://www.agora.io/cn/marketplace/cmeeting</t>
-  </si>
-  <si>
     <t>POPSTAGE —— Create your dream courses｜https://popstage.com/</t>
   </si>
   <si>
@@ -756,13 +750,7 @@
     <t>视频会议</t>
   </si>
   <si>
-    <t>开源项目 Jitsi Meet｜https://github.com/jitsi/jitsi-meet</t>
-  </si>
-  <si>
     <t>网络会议系统</t>
-  </si>
-  <si>
-    <t>开源项目 Bigbluebutton｜ https://github.com/bigbluebutton/bigbluebutton</t>
   </si>
   <si>
     <t>虚拟活动（Virtual Events）</t>
@@ -893,6 +881,101 @@
   <si>
     <t>开源项目 Zy Player｜https://github.com/cuiocean/ZY-Player</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cmeeting｜https://www.agora.io/cn/marketplace/cmeeting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room.Cafe｜https://github.com/aonesuite/room.cafe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微光｜http://www.vlightv.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metastream｜https://github.com/samuelmaddock/metastream</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Syncplay｜https ://github.com/Syncplay/syncplay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n.eko｜https://github.com/m1k1o/neko</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaddleBoBo｜https://github.com/JiehangXie/PaddleBoBo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hyperbeam｜https://hyperbeam.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collabedit丨https://collabedit.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeanywhere丨https://codeanywhere.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CodingView.io丨https://codingview.io/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowMeBug丨https://www.showmebug.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远程招聘（Online Interview）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>妙记多Mojidoc丨https://www.mojidoc.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpatialChat丨https://www.spatial.chat/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jitsi Meet｜https://github.com/jitsi/jitsi-meet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bigbluebutton｜ https://github.com/bigbluebutton/bigbluebutton</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视频会议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ehlo丨https://www.ehlo.space/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spot丨https://www.spotvirtual.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vertex Gallery 虚拟画廊｜https://vertexgallery.pavece.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infinite-Art-Gallery丨https://github.com/Brazil-0034/Infinite-Art-Gallery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kalidoface｜https://github.com/yeemachine/kalidokit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开源项目 Bigbluebutton｜ https://github.com/bigbluebutton/bigbluebutton</t>
   </si>
 </sst>
 </file>
@@ -1250,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D4BE62-C0D3-7340-A9ED-C3DB0E99B2E5}">
-  <dimension ref="A1:D237"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="C233" sqref="C233"/>
+    <sheetView tabSelected="1" topLeftCell="C156" workbookViewId="0">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1261,12 +1344,12 @@
     <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s">
         <v>203</v>
@@ -1275,7 +1358,7 @@
         <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1735,7 +1818,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>217</v>
       </c>
@@ -1746,7 +1829,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>217</v>
       </c>
@@ -1757,7 +1840,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>217</v>
       </c>
@@ -1768,7 +1851,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>217</v>
       </c>
@@ -1776,7 +1859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>217</v>
       </c>
@@ -1784,7 +1867,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>217</v>
       </c>
@@ -1792,7 +1875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>217</v>
       </c>
@@ -1800,7 +1883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>217</v>
       </c>
@@ -1808,7 +1891,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>217</v>
       </c>
@@ -1816,7 +1899,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -1827,7 +1910,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>217</v>
       </c>
@@ -1838,7 +1921,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>217</v>
       </c>
@@ -1846,10 +1929,10 @@
         <v>51</v>
       </c>
       <c r="C60" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>217</v>
       </c>
@@ -1857,64 +1940,76 @@
         <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>217</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>51</v>
+      </c>
+      <c r="C62" t="s">
+        <v>285</v>
+      </c>
+      <c r="D62">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>217</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>284</v>
+      </c>
+      <c r="D63">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C64" t="s">
-        <v>218</v>
+        <v>286</v>
+      </c>
+      <c r="D64">
+        <v>20220916</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C66" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
         <v>218</v>
@@ -1922,398 +2017,410 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
-      </c>
-      <c r="C68" t="s">
-        <v>229</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s">
         <v>227</v>
-      </c>
-      <c r="B69" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B71" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C71" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B72" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B73" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="C74" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
-      </c>
-      <c r="C77" t="s">
-        <v>233</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B78" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="C78" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="C79" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="C80" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="C81" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B82" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B84" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B85" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B86" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
-      </c>
-      <c r="C88" t="s">
-        <v>235</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B89" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B90" t="s">
-        <v>80</v>
-      </c>
-      <c r="C90" t="s">
-        <v>235</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B91" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>233</v>
+      </c>
+      <c r="B92" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" t="s">
         <v>234</v>
-      </c>
-      <c r="B92" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B93" t="s">
-        <v>236</v>
+        <v>78</v>
       </c>
       <c r="C93" t="s">
-        <v>237</v>
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>80</v>
+      </c>
+      <c r="C95" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="B98" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>235</v>
+      </c>
+      <c r="C98" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="B99" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>92</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>92</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>92</v>
       </c>
       <c r="B102" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>92</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>92</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>92</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>92</v>
       </c>
       <c r="B106" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>92</v>
       </c>
       <c r="B107" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>92</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>92</v>
       </c>
       <c r="B109" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>92</v>
       </c>
       <c r="B110" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>92</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>92</v>
       </c>
       <c r="B112" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2321,7 +2428,7 @@
         <v>92</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2329,7 +2436,7 @@
         <v>92</v>
       </c>
       <c r="B114" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2337,7 +2444,7 @@
         <v>92</v>
       </c>
       <c r="B115" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2345,7 +2452,7 @@
         <v>92</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2353,7 +2460,7 @@
         <v>92</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2361,7 +2468,7 @@
         <v>92</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2369,7 +2476,7 @@
         <v>92</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2377,7 +2484,7 @@
         <v>92</v>
       </c>
       <c r="B120" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2385,7 +2492,7 @@
         <v>92</v>
       </c>
       <c r="B121" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2393,47 +2500,47 @@
         <v>92</v>
       </c>
       <c r="B122" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B123" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B124" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2441,7 +2548,7 @@
         <v>121</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2449,7 +2556,7 @@
         <v>121</v>
       </c>
       <c r="B129" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2457,7 +2564,7 @@
         <v>121</v>
       </c>
       <c r="B130" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2465,7 +2572,7 @@
         <v>121</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2473,7 +2580,7 @@
         <v>121</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2481,7 +2588,7 @@
         <v>121</v>
       </c>
       <c r="B133" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2489,7 +2596,7 @@
         <v>121</v>
       </c>
       <c r="B134" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2497,7 +2604,7 @@
         <v>121</v>
       </c>
       <c r="B135" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2505,7 +2612,7 @@
         <v>121</v>
       </c>
       <c r="B136" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2513,7 +2620,7 @@
         <v>121</v>
       </c>
       <c r="B137" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2521,47 +2628,47 @@
         <v>121</v>
       </c>
       <c r="B138" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B139" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B140" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B143" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2569,7 +2676,7 @@
         <v>138</v>
       </c>
       <c r="B144" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2577,7 +2684,7 @@
         <v>138</v>
       </c>
       <c r="B145" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2585,7 +2692,7 @@
         <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2593,7 +2700,7 @@
         <v>138</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2601,7 +2708,7 @@
         <v>138</v>
       </c>
       <c r="B148" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2609,7 +2716,7 @@
         <v>138</v>
       </c>
       <c r="B149" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2617,7 +2724,7 @@
         <v>138</v>
       </c>
       <c r="B150" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2625,7 +2732,7 @@
         <v>138</v>
       </c>
       <c r="B151" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2633,7 +2740,7 @@
         <v>138</v>
       </c>
       <c r="B152" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2641,62 +2748,47 @@
         <v>138</v>
       </c>
       <c r="B153" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B154" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B155" t="s">
-        <v>156</v>
-      </c>
-      <c r="C155" t="s">
-        <v>238</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
-      </c>
-      <c r="C156" t="s">
-        <v>239</v>
-      </c>
-      <c r="D156">
-        <v>20220812</v>
+        <v>151</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>157</v>
-      </c>
-      <c r="C157" t="s">
-        <v>240</v>
-      </c>
-      <c r="D157">
-        <v>20220812</v>
+        <v>152</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2704,7 +2796,13 @@
         <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="C159" t="s">
+        <v>289</v>
+      </c>
+      <c r="D159">
+        <v>20220916</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2712,269 +2810,335 @@
         <v>154</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="C160" t="s">
+        <v>290</v>
+      </c>
+      <c r="D160">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>154</v>
       </c>
       <c r="B161" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="C161" t="s">
+        <v>294</v>
+      </c>
+      <c r="D161">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>154</v>
       </c>
       <c r="B162" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="C162" t="s">
+        <v>295</v>
+      </c>
+      <c r="D162">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>154</v>
       </c>
       <c r="B163" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
+        <v>155</v>
+      </c>
+      <c r="C163" t="s">
+        <v>299</v>
+      </c>
+      <c r="D163">
+        <v>20220829</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>154</v>
       </c>
       <c r="B164" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+        <v>156</v>
+      </c>
+      <c r="C164" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>154</v>
       </c>
       <c r="B165" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
       <c r="C165" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>282</v>
+      </c>
+      <c r="D165">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>154</v>
       </c>
       <c r="B166" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
+        <v>239</v>
+      </c>
+      <c r="C166" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>154</v>
       </c>
       <c r="B167" t="s">
-        <v>243</v>
+        <v>298</v>
       </c>
       <c r="C167" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B168" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
+        <v>157</v>
+      </c>
+      <c r="C168" t="s">
+        <v>237</v>
+      </c>
+      <c r="D168">
+        <v>20220812</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B169" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
+        <v>157</v>
+      </c>
+      <c r="C169" t="s">
+        <v>238</v>
+      </c>
+      <c r="D169">
+        <v>20220812</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B170" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
+        <v>158</v>
+      </c>
+      <c r="C170" t="s">
+        <v>291</v>
+      </c>
+      <c r="D170">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B171" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
+        <v>158</v>
+      </c>
+      <c r="C171" t="s">
+        <v>290</v>
+      </c>
+      <c r="D171">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B172" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
+        <v>293</v>
+      </c>
+      <c r="C172" t="s">
+        <v>292</v>
+      </c>
+      <c r="D172">
+        <v>20220916</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B173" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B174" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B175" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B176" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B177" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B178" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B179" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B180" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
+        <v>240</v>
+      </c>
+      <c r="C180" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
         <v>166</v>
       </c>
       <c r="B181" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
         <v>166</v>
       </c>
       <c r="B182" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>166</v>
       </c>
       <c r="B183" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
       <c r="A184" t="s">
         <v>166</v>
       </c>
       <c r="B184" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>166</v>
       </c>
       <c r="B185" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>166</v>
       </c>
       <c r="B186" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
         <v>166</v>
       </c>
       <c r="B187" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
         <v>166</v>
       </c>
       <c r="B188" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>166</v>
       </c>
       <c r="B189" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>166</v>
       </c>
       <c r="B190" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
         <v>166</v>
       </c>
       <c r="B191" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>166</v>
       </c>
       <c r="B192" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2982,7 +3146,7 @@
         <v>166</v>
       </c>
       <c r="B193" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2990,473 +3154,650 @@
         <v>166</v>
       </c>
       <c r="B194" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B195" t="s">
-        <v>194</v>
-      </c>
-      <c r="C195" t="s">
-        <v>246</v>
+        <v>181</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B196" t="s">
-        <v>194</v>
-      </c>
-      <c r="C196" t="s">
-        <v>247</v>
+        <v>182</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B197" t="s">
-        <v>195</v>
-      </c>
-      <c r="C197" t="s">
-        <v>246</v>
+        <v>183</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B198" t="s">
-        <v>195</v>
-      </c>
-      <c r="C198" t="s">
-        <v>247</v>
+        <v>184</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B199" t="s">
-        <v>196</v>
-      </c>
-      <c r="C199" t="s">
-        <v>246</v>
+        <v>185</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B200" t="s">
-        <v>86</v>
-      </c>
-      <c r="C200" t="s">
-        <v>248</v>
+        <v>186</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B201" t="s">
-        <v>90</v>
-      </c>
-      <c r="C201" t="s">
-        <v>248</v>
+        <v>187</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B202" t="s">
-        <v>197</v>
-      </c>
-      <c r="C202" t="s">
-        <v>249</v>
+        <v>188</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B203" t="s">
-        <v>250</v>
-      </c>
-      <c r="C203" t="s">
-        <v>249</v>
+        <v>189</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B204" t="s">
-        <v>201</v>
-      </c>
-      <c r="C204" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B205" t="s">
-        <v>201</v>
-      </c>
-      <c r="C205" t="s">
-        <v>252</v>
+        <v>191</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B206" t="s">
-        <v>201</v>
-      </c>
-      <c r="C206" t="s">
-        <v>253</v>
+        <v>192</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="B207" t="s">
-        <v>201</v>
-      </c>
-      <c r="C207" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B208" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C208" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B209" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C209" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B210" t="s">
-        <v>255</v>
+        <v>195</v>
       </c>
       <c r="C210" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B211" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C211" t="s">
-        <v>257</v>
+        <v>243</v>
+      </c>
+      <c r="D211">
+        <v>20220829</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B212" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C212" t="s">
-        <v>258</v>
+        <v>301</v>
       </c>
       <c r="D212">
-        <v>20220812</v>
+        <v>20220829</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B213" t="s">
-        <v>84</v>
+        <v>196</v>
+      </c>
+      <c r="C213" t="s">
+        <v>302</v>
+      </c>
+      <c r="D213">
+        <v>20220829</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B214" t="s">
-        <v>85</v>
+        <v>196</v>
+      </c>
+      <c r="C214" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B215" t="s">
-        <v>200</v>
+        <v>86</v>
+      </c>
+      <c r="C215" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B216" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="C216" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B217" t="s">
-        <v>88</v>
+        <v>197</v>
+      </c>
+      <c r="C217" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B218" t="s">
-        <v>89</v>
+        <v>197</v>
+      </c>
+      <c r="C218" t="s">
+        <v>299</v>
+      </c>
+      <c r="D218">
+        <v>20220829</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B219" t="s">
-        <v>199</v>
+        <v>197</v>
+      </c>
+      <c r="C219" t="s">
+        <v>300</v>
+      </c>
+      <c r="D219">
+        <v>20220812</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B220" t="s">
-        <v>198</v>
+        <v>246</v>
+      </c>
+      <c r="C220" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B221" t="s">
-        <v>91</v>
+        <v>201</v>
+      </c>
+      <c r="C221" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B222" t="s">
-        <v>261</v>
+        <v>201</v>
+      </c>
+      <c r="C222" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B223" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C223" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B224" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C224" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B225" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C225" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B226" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C226" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B227" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C227" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B228" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C228" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B229" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C229" t="s">
-        <v>269</v>
+        <v>254</v>
+      </c>
+      <c r="D229">
+        <v>20220812</v>
       </c>
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B230" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="C230" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="D230">
-        <v>20220819</v>
+        <v>20220829</v>
       </c>
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B231" t="s">
-        <v>262</v>
-      </c>
-      <c r="C231" t="s">
-        <v>279</v>
-      </c>
-      <c r="D231">
-        <v>20220819</v>
+        <v>84</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B232" t="s">
-        <v>262</v>
-      </c>
-      <c r="C232" t="s">
-        <v>283</v>
-      </c>
-      <c r="D232">
-        <v>20220826</v>
+        <v>85</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B233" t="s">
-        <v>262</v>
-      </c>
-      <c r="C233" t="s">
-        <v>284</v>
-      </c>
-      <c r="D233">
-        <v>20220826</v>
+        <v>200</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B234" t="s">
-        <v>277</v>
-      </c>
-      <c r="C234" t="s">
-        <v>280</v>
-      </c>
-      <c r="D234">
-        <v>20220819</v>
+        <v>87</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B235" t="s">
-        <v>270</v>
-      </c>
-      <c r="C235" t="s">
-        <v>271</v>
+        <v>88</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B236" t="s">
-        <v>272</v>
-      </c>
-      <c r="C236" t="s">
-        <v>273</v>
-      </c>
-      <c r="D236">
-        <v>20220812</v>
+        <v>89</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
+        <v>256</v>
+      </c>
+      <c r="B237" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238" t="s">
+        <v>256</v>
+      </c>
+      <c r="B238" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" t="s">
+        <v>256</v>
+      </c>
+      <c r="B239" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" t="s">
+        <v>256</v>
+      </c>
+      <c r="B240" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" t="s">
+        <v>256</v>
+      </c>
+      <c r="B241" t="s">
+        <v>258</v>
+      </c>
+      <c r="C241" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242" t="s">
+        <v>256</v>
+      </c>
+      <c r="B242" t="s">
+        <v>258</v>
+      </c>
+      <c r="C242" t="s">
         <v>260</v>
       </c>
-      <c r="B237" t="s">
-        <v>281</v>
-      </c>
-      <c r="C237" t="s">
-        <v>282</v>
-      </c>
-      <c r="D237">
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" t="s">
+        <v>256</v>
+      </c>
+      <c r="B243" t="s">
+        <v>258</v>
+      </c>
+      <c r="C243" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" t="s">
+        <v>256</v>
+      </c>
+      <c r="B244" t="s">
+        <v>258</v>
+      </c>
+      <c r="C244" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" t="s">
+        <v>256</v>
+      </c>
+      <c r="B245" t="s">
+        <v>258</v>
+      </c>
+      <c r="C245" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" t="s">
+        <v>256</v>
+      </c>
+      <c r="B246" t="s">
+        <v>258</v>
+      </c>
+      <c r="C246" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247" t="s">
+        <v>256</v>
+      </c>
+      <c r="B247" t="s">
+        <v>258</v>
+      </c>
+      <c r="C247" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248" t="s">
+        <v>256</v>
+      </c>
+      <c r="B248" t="s">
+        <v>258</v>
+      </c>
+      <c r="C248" t="s">
+        <v>274</v>
+      </c>
+      <c r="D248">
+        <v>20220819</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" t="s">
+        <v>256</v>
+      </c>
+      <c r="B249" t="s">
+        <v>258</v>
+      </c>
+      <c r="C249" t="s">
+        <v>275</v>
+      </c>
+      <c r="D249">
+        <v>20220819</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250" t="s">
+        <v>256</v>
+      </c>
+      <c r="B250" t="s">
+        <v>258</v>
+      </c>
+      <c r="C250" t="s">
+        <v>279</v>
+      </c>
+      <c r="D250">
+        <v>20220826</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" t="s">
+        <v>256</v>
+      </c>
+      <c r="B251" t="s">
+        <v>258</v>
+      </c>
+      <c r="C251" t="s">
+        <v>280</v>
+      </c>
+      <c r="D251">
+        <v>20220826</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" t="s">
+        <v>256</v>
+      </c>
+      <c r="B252" t="s">
+        <v>273</v>
+      </c>
+      <c r="C252" t="s">
+        <v>276</v>
+      </c>
+      <c r="D252">
+        <v>20220819</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" t="s">
+        <v>256</v>
+      </c>
+      <c r="B253" t="s">
+        <v>266</v>
+      </c>
+      <c r="C253" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" t="s">
+        <v>256</v>
+      </c>
+      <c r="B254" t="s">
+        <v>268</v>
+      </c>
+      <c r="C254" t="s">
+        <v>269</v>
+      </c>
+      <c r="D254">
+        <v>20220812</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" t="s">
+        <v>256</v>
+      </c>
+      <c r="B255" t="s">
+        <v>277</v>
+      </c>
+      <c r="C255" t="s">
+        <v>278</v>
+      </c>
+      <c r="D255">
         <v>20220826</v>
       </c>
     </row>

</xml_diff>